<commit_message>
7.5.5版本的跟进更新【An Update following v7.5.5】
调整了国服比赛服的描述，并同步到Excel表格中。
Adjusted the descriptions of the Chinese tournament server. These changes are synchronized in the Excel workbook.
另外，改进了调试脚本的启动提示。现在，即使用户没有登录，也能正常使用该脚本。
Besides, improved the prompts on launch of Customized Program 03. Now, even if the user doesn't log in,
he/she can still use this program as normal.
</commit_message>
<xml_diff>
--- a/国服服务器列表.xlsx
+++ b/国服服务器列表.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\19250\Documents\GitHub\LoL-DIY-Programs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18C1C7C4-CD46-44E0-A369-DCCBD98F6EA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B298B4B-8013-4C7B-9184-CBD04A0EE9D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{8B27E1A9-18C2-4F7A-9B32-BAFDEA5E4F5B}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="83">
   <si>
     <t>艾欧尼亚</t>
   </si>
@@ -285,6 +285,22 @@
   </si>
   <si>
     <t>CQ100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FORCES</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>艾欧尼亚</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ionia</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>比赛服（Tournament）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -353,9 +369,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 主题">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -393,7 +409,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -499,7 +515,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -641,7 +657,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -649,7 +665,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEC4D7EB-5F6A-4227-9205-BFADD3F1FF57}">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1081,6 +1097,20 @@
         <v>70</v>
       </c>
     </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>82</v>
+      </c>
+      <c r="B31" t="s">
+        <v>80</v>
+      </c>
+      <c r="C31" t="s">
+        <v>81</v>
+      </c>
+      <c r="D31" t="s">
+        <v>79</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:D30" xr:uid="{CEC4D7EB-5F6A-4227-9205-BFADD3F1FF57}"/>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>